<commit_message>
Demo descriptions and project links
</commit_message>
<xml_diff>
--- a/doc/demo/schemas24a/sparql_endpoints.xlsx
+++ b/doc/demo/schemas24a/sparql_endpoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\K\Meteor\viziquer_2\doc\demo\schemas24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\K\Meteor\viziquer_2\doc\demo\schemas24a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013EE3EE-F8B3-4945-BB5B-1D0A9DBA97BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73202D01-4A07-47D9-B6D1-744211EEA2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8820" yWindow="5940" windowWidth="46050" windowHeight="23925" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10935" yWindow="7605" windowWidth="42000" windowHeight="21945" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Linked_data_Endpoints" sheetId="1" r:id="rId1"/>
@@ -1244,7 +1244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1318,27 +1318,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4830,7 +4811,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4889,10 +4872,10 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>288</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="C2" t="s">
         <v>290</v>
@@ -4900,271 +4883,267 @@
       <c r="D2" t="s">
         <v>201</v>
       </c>
-      <c r="E2" s="1">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1">
-        <v>757</v>
-      </c>
-      <c r="G2" s="1">
-        <v>46</v>
+      <c r="E2" s="13">
+        <v>2</v>
+      </c>
+      <c r="F2" s="9">
+        <v>1757437</v>
+      </c>
+      <c r="G2" s="9">
+        <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>342</v>
+        <v>255</v>
       </c>
       <c r="J2" t="s">
-        <v>298</v>
+        <v>244</v>
       </c>
       <c r="K2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" s="29" customFormat="1">
-      <c r="A3" s="29" t="s">
-        <v>212</v>
-      </c>
-      <c r="B3" s="29" t="s">
+      <c r="M2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
         <v>338</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" t="s">
         <v>290</v>
       </c>
-      <c r="D3" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E3" s="35">
-        <v>2</v>
-      </c>
-      <c r="F3" s="33">
-        <v>1757437</v>
-      </c>
-      <c r="G3" s="33">
-        <v>14</v>
-      </c>
-      <c r="I3" s="29" t="s">
-        <v>255</v>
-      </c>
-      <c r="J3" s="29" t="s">
+      <c r="D3" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1263</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="J3" t="s">
+        <v>298</v>
+      </c>
+      <c r="K3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" t="s">
+        <v>338</v>
+      </c>
+      <c r="C4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2637168</v>
+      </c>
+      <c r="G4" s="1">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
+        <v>266</v>
+      </c>
+      <c r="J4" t="s">
+        <v>294</v>
+      </c>
+      <c r="K4" t="s">
+        <v>245</v>
+      </c>
+      <c r="M4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="1">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>283</v>
+      </c>
+      <c r="J5" t="s">
+        <v>298</v>
+      </c>
+      <c r="K5" t="s">
+        <v>245</v>
+      </c>
+      <c r="M5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6" t="s">
+        <v>338</v>
+      </c>
+      <c r="C6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D6" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" s="15">
+        <v>6</v>
+      </c>
+      <c r="F6" s="9">
+        <v>21042948</v>
+      </c>
+      <c r="G6" s="9">
+        <v>67</v>
+      </c>
+      <c r="I6" t="s">
+        <v>274</v>
+      </c>
+      <c r="J6" t="s">
         <v>244</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K6" t="s">
         <v>245</v>
       </c>
-      <c r="L3" s="32"/>
-      <c r="M3" s="29" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="29" customFormat="1">
-      <c r="A4" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" s="29" t="s">
+      <c r="M6" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" t="s">
         <v>338</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C7" t="s">
         <v>290</v>
       </c>
-      <c r="D4" s="36" t="s">
-        <v>201</v>
-      </c>
-      <c r="E4" s="30">
-        <v>3</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="G4" s="30">
-        <v>1263</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="J4" s="29" t="s">
-        <v>298</v>
-      </c>
-      <c r="K4" s="29" t="s">
+      <c r="D7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" s="1">
+        <v>7</v>
+      </c>
+      <c r="F7" s="9">
+        <v>5014</v>
+      </c>
+      <c r="G7" s="9">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>246</v>
+      </c>
+      <c r="J7" t="s">
+        <v>244</v>
+      </c>
+      <c r="K7" t="s">
         <v>245</v>
       </c>
-      <c r="L4" s="32"/>
-    </row>
-    <row r="5" spans="1:14" s="29" customFormat="1">
-      <c r="A5" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="B5" s="29" t="s">
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
         <v>338</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C8" t="s">
         <v>290</v>
       </c>
-      <c r="D5" s="36" t="s">
-        <v>201</v>
-      </c>
-      <c r="E5" s="30">
-        <v>3</v>
-      </c>
-      <c r="F5" s="30">
-        <v>2637168</v>
-      </c>
-      <c r="G5" s="30">
-        <v>37</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>266</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>294</v>
-      </c>
-      <c r="K5" s="29" t="s">
+      <c r="D8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E8" s="1">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="1">
+        <v>47</v>
+      </c>
+      <c r="I8" t="s">
+        <v>250</v>
+      </c>
+      <c r="J8" t="s">
+        <v>296</v>
+      </c>
+      <c r="K8" t="s">
         <v>245</v>
       </c>
-      <c r="L5" s="32"/>
-      <c r="M5" s="29" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="29" customFormat="1">
-      <c r="A6" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6" s="29" t="s">
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" t="s">
         <v>338</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C9" t="s">
         <v>290</v>
       </c>
-      <c r="D6" s="36" t="s">
-        <v>201</v>
-      </c>
-      <c r="E6" s="30">
-        <v>3</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="G6" s="30">
-        <v>17</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>283</v>
-      </c>
-      <c r="J6" s="29" t="s">
-        <v>298</v>
-      </c>
-      <c r="K6" s="29" t="s">
+      <c r="D9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" s="10">
+        <v>9</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1718004</v>
+      </c>
+      <c r="G9" s="9">
+        <v>52</v>
+      </c>
+      <c r="I9" t="s">
+        <v>249</v>
+      </c>
+      <c r="J9" t="s">
+        <v>244</v>
+      </c>
+      <c r="K9" t="s">
         <v>245</v>
       </c>
-      <c r="L6" s="32"/>
-      <c r="M6" s="29" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="29" customFormat="1">
-      <c r="A7" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>338</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E7" s="37">
-        <v>6</v>
-      </c>
-      <c r="F7" s="33">
-        <v>21042948</v>
-      </c>
-      <c r="G7" s="33">
-        <v>67</v>
-      </c>
-      <c r="I7" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="J7" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="K7" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="L7" s="32"/>
-      <c r="M7" s="29" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="29" customFormat="1">
-      <c r="A8" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>338</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E8" s="30">
-        <v>7</v>
-      </c>
-      <c r="F8" s="33">
-        <v>5014</v>
-      </c>
-      <c r="G8" s="33">
-        <v>20</v>
-      </c>
-      <c r="I8" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="K8" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="L8" s="32"/>
-    </row>
-    <row r="9" spans="1:14" s="29" customFormat="1">
-      <c r="A9" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>338</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E9" s="30">
-        <v>7</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="30">
-        <v>47</v>
-      </c>
-      <c r="I9" s="29" t="s">
-        <v>250</v>
-      </c>
-      <c r="J9" s="29" t="s">
-        <v>296</v>
-      </c>
-      <c r="K9" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="L9" s="32"/>
+      <c r="M9" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
         <v>338</v>
@@ -5175,31 +5154,31 @@
       <c r="D10" t="s">
         <v>201</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="1">
         <v>9</v>
       </c>
       <c r="F10" s="9">
-        <v>1718004</v>
+        <v>19809666</v>
       </c>
       <c r="G10" s="9">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="J10" t="s">
-        <v>244</v>
+        <v>296</v>
       </c>
       <c r="K10" t="s">
         <v>245</v>
       </c>
       <c r="M10" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>214</v>
       </c>
       <c r="B11" t="s">
         <v>338</v>
@@ -5211,30 +5190,27 @@
         <v>201</v>
       </c>
       <c r="E11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F11" s="9">
-        <v>19809666</v>
+        <v>12396</v>
       </c>
       <c r="G11" s="9">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="I11" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="J11" t="s">
-        <v>296</v>
+        <v>244</v>
       </c>
       <c r="K11" t="s">
         <v>245</v>
       </c>
-      <c r="M11" t="s">
-        <v>312</v>
-      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>214</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
         <v>338</v>
@@ -5246,16 +5222,19 @@
         <v>201</v>
       </c>
       <c r="E12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F12" s="9">
-        <v>12396</v>
+        <v>13737813</v>
       </c>
       <c r="G12" s="9">
-        <v>60</v>
+        <v>34</v>
+      </c>
+      <c r="H12" t="s">
+        <v>208</v>
       </c>
       <c r="I12" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="J12" t="s">
         <v>244</v>
@@ -5263,13 +5242,16 @@
       <c r="K12" t="s">
         <v>245</v>
       </c>
+      <c r="M12" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>288</v>
       </c>
       <c r="B13" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="C13" t="s">
         <v>290</v>
@@ -5278,28 +5260,22 @@
         <v>201</v>
       </c>
       <c r="E13" s="1">
-        <v>11</v>
-      </c>
-      <c r="F13" s="9">
-        <v>13737813</v>
-      </c>
-      <c r="G13" s="9">
-        <v>34</v>
-      </c>
-      <c r="H13" t="s">
-        <v>208</v>
+        <v>13</v>
+      </c>
+      <c r="F13" s="1">
+        <v>757</v>
+      </c>
+      <c r="G13" s="1">
+        <v>46</v>
       </c>
       <c r="I13" t="s">
-        <v>252</v>
+        <v>342</v>
       </c>
       <c r="J13" t="s">
-        <v>244</v>
+        <v>298</v>
       </c>
       <c r="K13" t="s">
         <v>245</v>
-      </c>
-      <c r="M13" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -5410,79 +5386,81 @@
         <v>290</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
-      <c r="A17" t="s">
+    <row r="17" spans="1:14" ht="30">
+      <c r="A17" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="E17" s="22">
+        <v>15</v>
+      </c>
+      <c r="F17" s="22">
+        <v>6148355</v>
+      </c>
+      <c r="G17" s="22">
+        <v>57</v>
+      </c>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="M17" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="N17" s="21"/>
+    </row>
+    <row r="18" spans="1:14" ht="30">
+      <c r="A18" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="E18" s="25">
+        <v>16</v>
+      </c>
+      <c r="F18" s="23">
+        <v>93698</v>
+      </c>
+      <c r="G18" s="23">
+        <v>53</v>
+      </c>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="L18" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="M18" s="21" t="s">
+        <v>348</v>
+      </c>
+      <c r="N18" s="21"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" t="s">
         <v>235</v>
-      </c>
-      <c r="B17" t="s">
-        <v>338</v>
-      </c>
-      <c r="C17" t="s">
-        <v>290</v>
-      </c>
-      <c r="D17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E17" s="1">
-        <v>18</v>
-      </c>
-      <c r="F17" s="9">
-        <v>65749349</v>
-      </c>
-      <c r="G17" s="16">
-        <v>163</v>
-      </c>
-      <c r="I17" t="s">
-        <v>279</v>
-      </c>
-      <c r="J17" t="s">
-        <v>244</v>
-      </c>
-      <c r="K17" t="s">
-        <v>245</v>
-      </c>
-      <c r="M17" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
-      <c r="A18" t="s">
-        <v>162</v>
-      </c>
-      <c r="B18" t="s">
-        <v>338</v>
-      </c>
-      <c r="C18" t="s">
-        <v>290</v>
-      </c>
-      <c r="D18" t="s">
-        <v>201</v>
-      </c>
-      <c r="E18" s="1">
-        <v>19</v>
-      </c>
-      <c r="F18" s="1">
-        <v>611</v>
-      </c>
-      <c r="G18" s="1">
-        <v>115</v>
-      </c>
-      <c r="I18" t="s">
-        <v>262</v>
-      </c>
-      <c r="J18" t="s">
-        <v>298</v>
-      </c>
-      <c r="K18" t="s">
-        <v>245</v>
-      </c>
-      <c r="M18" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" t="s">
-        <v>179</v>
       </c>
       <c r="B19" t="s">
         <v>338</v>
@@ -5494,350 +5472,341 @@
         <v>201</v>
       </c>
       <c r="E19" s="1">
-        <v>20</v>
-      </c>
-      <c r="F19" s="1">
-        <v>137133007</v>
-      </c>
-      <c r="G19" s="1">
-        <v>139</v>
+        <v>18</v>
+      </c>
+      <c r="F19" s="9">
+        <v>65749349</v>
+      </c>
+      <c r="G19" s="16">
+        <v>163</v>
       </c>
       <c r="I19" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="J19" t="s">
-        <v>294</v>
+        <v>244</v>
       </c>
       <c r="K19" t="s">
         <v>245</v>
       </c>
       <c r="M19" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="30">
+      <c r="A20" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="E20" s="25">
+        <v>18</v>
+      </c>
+      <c r="F20" s="25">
+        <v>1689698</v>
+      </c>
+      <c r="G20" s="25">
+        <v>43</v>
+      </c>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="K20" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>343</v>
+      </c>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" t="s">
+        <v>338</v>
+      </c>
+      <c r="C21" t="s">
+        <v>290</v>
+      </c>
+      <c r="D21" t="s">
+        <v>201</v>
+      </c>
+      <c r="E21" s="1">
+        <v>19</v>
+      </c>
+      <c r="F21" s="1">
+        <v>611</v>
+      </c>
+      <c r="G21" s="1">
+        <v>115</v>
+      </c>
+      <c r="I21" t="s">
+        <v>262</v>
+      </c>
+      <c r="J21" t="s">
+        <v>298</v>
+      </c>
+      <c r="K21" t="s">
+        <v>245</v>
+      </c>
+      <c r="M21" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" t="s">
+        <v>179</v>
+      </c>
+      <c r="B22" t="s">
+        <v>338</v>
+      </c>
+      <c r="C22" t="s">
+        <v>290</v>
+      </c>
+      <c r="D22" t="s">
+        <v>201</v>
+      </c>
+      <c r="E22" s="1">
+        <v>20</v>
+      </c>
+      <c r="F22" s="1">
+        <v>137133007</v>
+      </c>
+      <c r="G22" s="1">
+        <v>139</v>
+      </c>
+      <c r="I22" t="s">
+        <v>278</v>
+      </c>
+      <c r="J22" t="s">
+        <v>294</v>
+      </c>
+      <c r="K22" t="s">
+        <v>245</v>
+      </c>
+      <c r="M22" t="s">
         <v>320</v>
       </c>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-    </row>
-    <row r="20" spans="1:16" s="29" customFormat="1">
-      <c r="A20" s="29" t="s">
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B23" t="s">
         <v>338</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C23" t="s">
         <v>290</v>
       </c>
-      <c r="D20" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E20" s="30">
+      <c r="D23" t="s">
+        <v>201</v>
+      </c>
+      <c r="E23" s="1">
         <v>20</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F23" s="1">
         <v>5761781</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G23" s="1">
         <v>55</v>
       </c>
-      <c r="I20" s="29" t="s">
+      <c r="I23" t="s">
         <v>282</v>
       </c>
-      <c r="J20" s="29" t="s">
+      <c r="J23" t="s">
         <v>298</v>
       </c>
-      <c r="K20" s="29" t="s">
+      <c r="K23" t="s">
         <v>245</v>
       </c>
-      <c r="L20" s="32"/>
-      <c r="M20" s="29" t="s">
+      <c r="M23" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="29" customFormat="1">
-      <c r="A21" s="29" t="s">
+    <row r="24" spans="1:14">
+      <c r="A24" t="s">
         <v>204</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B24" t="s">
         <v>338</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C24" t="s">
         <v>290</v>
       </c>
-      <c r="D21" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E21" s="30">
+      <c r="D24" t="s">
+        <v>201</v>
+      </c>
+      <c r="E24" s="1">
         <v>21</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F24" s="9">
         <v>101262</v>
       </c>
-      <c r="G21" s="33">
+      <c r="G24" s="9">
         <v>127</v>
       </c>
-      <c r="I21" s="29" t="s">
+      <c r="I24" t="s">
         <v>247</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J24" t="s">
         <v>244</v>
       </c>
-      <c r="K21" s="29" t="s">
+      <c r="K24" t="s">
         <v>245</v>
       </c>
-      <c r="L21" s="32"/>
-      <c r="M21" s="29" t="s">
+      <c r="M24" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="29" customFormat="1">
-      <c r="A22" s="29" t="s">
+    <row r="25" spans="1:14">
+      <c r="A25" t="s">
         <v>213</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B25" t="s">
         <v>338</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C25" t="s">
         <v>290</v>
       </c>
-      <c r="D22" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E22" s="30">
+      <c r="D25" t="s">
+        <v>201</v>
+      </c>
+      <c r="E25" s="1">
         <v>21</v>
       </c>
-      <c r="F22" s="33">
+      <c r="F25" s="9">
         <v>1352654</v>
       </c>
-      <c r="G22" s="33">
+      <c r="G25" s="9">
         <v>48</v>
       </c>
-      <c r="I22" s="29" t="s">
+      <c r="I25" t="s">
         <v>257</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="J25" t="s">
         <v>244</v>
       </c>
-      <c r="K22" s="29" t="s">
+      <c r="K25" t="s">
         <v>245</v>
       </c>
-      <c r="L22" s="32"/>
-    </row>
-    <row r="23" spans="1:16" s="29" customFormat="1">
-      <c r="A23" s="29" t="s">
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" t="s">
         <v>178</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B26" t="s">
         <v>338</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C26" t="s">
         <v>290</v>
       </c>
-      <c r="D23" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E23" s="30">
+      <c r="D26" t="s">
+        <v>201</v>
+      </c>
+      <c r="E26" s="1">
         <v>21</v>
       </c>
-      <c r="F23" s="30">
+      <c r="F26" s="1">
         <v>325600</v>
       </c>
-      <c r="G23" s="30">
+      <c r="G26" s="1">
         <v>153</v>
       </c>
-      <c r="I23" s="29" t="s">
+      <c r="I26" t="s">
         <v>267</v>
       </c>
-      <c r="J23" s="29" t="s">
+      <c r="J26" t="s">
         <v>294</v>
       </c>
-      <c r="K23" s="29" t="s">
+      <c r="K26" t="s">
         <v>245</v>
       </c>
-      <c r="L23" s="32"/>
-      <c r="M23" s="29" t="s">
+      <c r="M26" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="29" customFormat="1">
-      <c r="A24" s="29" t="s">
+    <row r="27" spans="1:14">
+      <c r="A27" t="s">
         <v>176</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B27" t="s">
         <v>338</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C27" t="s">
         <v>290</v>
       </c>
-      <c r="D24" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E24" s="30">
+      <c r="D27" t="s">
+        <v>201</v>
+      </c>
+      <c r="E27" s="1">
         <v>22</v>
       </c>
-      <c r="F24" s="30">
+      <c r="F27" s="1">
         <v>34279</v>
       </c>
-      <c r="G24" s="30">
+      <c r="G27" s="1">
         <v>130</v>
       </c>
-      <c r="I24" s="29" t="s">
+      <c r="I27" t="s">
         <v>280</v>
       </c>
-      <c r="J24" s="29" t="s">
+      <c r="J27" t="s">
         <v>294</v>
       </c>
-      <c r="K24" s="29" t="s">
+      <c r="K27" t="s">
         <v>245</v>
       </c>
-      <c r="L24" s="32"/>
-      <c r="M24" s="34" t="s">
+      <c r="M27" s="29" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="29" customFormat="1">
-      <c r="A25" s="29" t="s">
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
         <v>177</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B28" t="s">
         <v>338</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C28" t="s">
         <v>290</v>
       </c>
-      <c r="D25" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E25" s="30">
+      <c r="D28" t="s">
+        <v>201</v>
+      </c>
+      <c r="E28" s="1">
         <v>22</v>
       </c>
-      <c r="F25" s="30">
+      <c r="F28" s="1">
         <v>59640</v>
       </c>
-      <c r="G25" s="30">
+      <c r="G28" s="1">
         <v>125</v>
       </c>
-      <c r="I25" s="29" t="s">
+      <c r="I28" t="s">
         <v>286</v>
       </c>
-      <c r="J25" s="29" t="s">
+      <c r="J28" t="s">
         <v>294</v>
       </c>
-      <c r="K25" s="29" t="s">
+      <c r="K28" t="s">
         <v>245</v>
       </c>
-      <c r="L25" s="32"/>
-      <c r="M25" s="29" t="s">
+      <c r="M28" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="29" customFormat="1">
-      <c r="A26" s="29" t="s">
+    <row r="29" spans="1:14">
+      <c r="A29" t="s">
         <v>211</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>338</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E26" s="30">
-        <v>23</v>
-      </c>
-      <c r="F26" s="33">
-        <v>29767602</v>
-      </c>
-      <c r="G26" s="33">
-        <v>185</v>
-      </c>
-      <c r="I26" s="29" t="s">
-        <v>350</v>
-      </c>
-      <c r="J26" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="K26" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="L26" s="32"/>
-    </row>
-    <row r="27" spans="1:16" s="29" customFormat="1">
-      <c r="A27" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>338</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E27" s="30">
-        <v>23</v>
-      </c>
-      <c r="F27" s="30">
-        <v>20238500</v>
-      </c>
-      <c r="G27" s="30">
-        <v>142</v>
-      </c>
-      <c r="I27" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="J27" s="29" t="s">
-        <v>294</v>
-      </c>
-      <c r="K27" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="L27" s="32"/>
-      <c r="M27" s="34" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" s="29" customFormat="1">
-      <c r="A28" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="B28" s="29" t="s">
-        <v>338</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E28" s="30">
-        <v>23</v>
-      </c>
-      <c r="F28" s="29">
-        <v>2482114</v>
-      </c>
-      <c r="G28" s="29">
-        <v>74</v>
-      </c>
-      <c r="I28" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="J28" s="29" t="s">
-        <v>294</v>
-      </c>
-      <c r="K28" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="L28" s="32"/>
-      <c r="M28" s="29" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
-      <c r="A29" t="s">
-        <v>160</v>
       </c>
       <c r="B29" t="s">
         <v>338</v>
@@ -5849,32 +5818,27 @@
         <v>201</v>
       </c>
       <c r="E29" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F29" s="9">
-        <v>8152</v>
+        <v>29767602</v>
       </c>
       <c r="G29" s="9">
-        <v>127</v>
+        <v>185</v>
       </c>
       <c r="I29" t="s">
-        <v>263</v>
+        <v>350</v>
       </c>
       <c r="J29" t="s">
-        <v>296</v>
+        <v>244</v>
       </c>
       <c r="K29" t="s">
         <v>245</v>
       </c>
-      <c r="M29" t="s">
-        <v>318</v>
-      </c>
-      <c r="O29" s="29"/>
-      <c r="P29" s="29"/>
-    </row>
-    <row r="30" spans="1:16">
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>175</v>
       </c>
       <c r="B30" t="s">
         <v>338</v>
@@ -5886,32 +5850,30 @@
         <v>201</v>
       </c>
       <c r="E30" s="1">
-        <v>24</v>
-      </c>
-      <c r="F30" s="9">
-        <v>6230572</v>
-      </c>
-      <c r="G30" s="9">
-        <v>68</v>
+        <v>23</v>
+      </c>
+      <c r="F30" s="1">
+        <v>20238500</v>
+      </c>
+      <c r="G30" s="1">
+        <v>142</v>
       </c>
       <c r="I30" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="J30" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K30" t="s">
         <v>245</v>
       </c>
-      <c r="M30" t="s">
-        <v>322</v>
-      </c>
-      <c r="O30" s="29"/>
-      <c r="P30" s="29"/>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="M30" s="29" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>236</v>
+        <v>194</v>
       </c>
       <c r="B31" t="s">
         <v>338</v>
@@ -5923,29 +5885,30 @@
         <v>201</v>
       </c>
       <c r="E31" s="1">
-        <v>25</v>
-      </c>
-      <c r="F31" s="9">
-        <v>9677</v>
-      </c>
-      <c r="G31" s="9">
-        <v>132</v>
+        <v>23</v>
+      </c>
+      <c r="F31">
+        <v>2482114</v>
+      </c>
+      <c r="G31">
+        <v>74</v>
       </c>
       <c r="I31" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="J31" t="s">
-        <v>244</v>
+        <v>294</v>
       </c>
       <c r="K31" t="s">
         <v>245</v>
       </c>
-      <c r="O31" s="29"/>
-      <c r="P31" s="29"/>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="M31" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>160</v>
       </c>
       <c r="B32" t="s">
         <v>338</v>
@@ -5956,17 +5919,17 @@
       <c r="D32" t="s">
         <v>201</v>
       </c>
-      <c r="E32" s="12">
-        <v>28</v>
+      <c r="E32" s="1">
+        <v>24</v>
       </c>
       <c r="F32" s="9">
-        <v>255521795</v>
+        <v>8152</v>
       </c>
       <c r="G32" s="9">
-        <v>328</v>
+        <v>127</v>
       </c>
       <c r="I32" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="J32" t="s">
         <v>296</v>
@@ -5975,14 +5938,12 @@
         <v>245</v>
       </c>
       <c r="M32" t="s">
-        <v>303</v>
-      </c>
-      <c r="O32" s="29"/>
-      <c r="P32" s="29"/>
+        <v>318</v>
+      </c>
     </row>
     <row r="33" spans="1:16">
       <c r="A33" t="s">
-        <v>238</v>
+        <v>115</v>
       </c>
       <c r="B33" t="s">
         <v>338</v>
@@ -5994,66 +5955,68 @@
         <v>201</v>
       </c>
       <c r="E33" s="1">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F33" s="9">
-        <v>116198466</v>
+        <v>6230572</v>
       </c>
       <c r="G33" s="9">
-        <v>176</v>
+        <v>68</v>
       </c>
       <c r="I33" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="J33" t="s">
-        <v>244</v>
+        <v>296</v>
       </c>
       <c r="K33" t="s">
         <v>245</v>
       </c>
       <c r="M33" t="s">
-        <v>331</v>
-      </c>
-      <c r="O33" s="29"/>
-      <c r="P33" s="29"/>
-    </row>
-    <row r="34" spans="1:16">
-      <c r="A34" t="s">
-        <v>271</v>
-      </c>
-      <c r="B34" t="s">
-        <v>338</v>
-      </c>
-      <c r="C34" t="s">
-        <v>290</v>
-      </c>
-      <c r="D34" t="s">
-        <v>201</v>
-      </c>
-      <c r="E34" s="1">
-        <v>30</v>
-      </c>
-      <c r="F34" s="1">
-        <v>37093353</v>
-      </c>
-      <c r="G34" s="1">
-        <v>59</v>
-      </c>
-      <c r="I34" t="s">
-        <v>272</v>
-      </c>
-      <c r="J34" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="30">
+      <c r="A34" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="E34" s="25">
+        <v>24</v>
+      </c>
+      <c r="F34" s="23">
+        <v>233836</v>
+      </c>
+      <c r="G34" s="23">
+        <v>106</v>
+      </c>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="K34" t="s">
-        <v>245</v>
-      </c>
-      <c r="O34" s="29"/>
-      <c r="P34" s="29"/>
+      <c r="K34" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="L34" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="M34" s="21" t="s">
+        <v>313</v>
+      </c>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="21"/>
     </row>
     <row r="35" spans="1:16">
       <c r="A35" t="s">
-        <v>0</v>
+        <v>236</v>
       </c>
       <c r="B35" t="s">
         <v>338</v>
@@ -6064,67 +6027,64 @@
       <c r="D35" t="s">
         <v>201</v>
       </c>
-      <c r="E35" s="10">
-        <v>32</v>
+      <c r="E35" s="1">
+        <v>25</v>
       </c>
       <c r="F35" s="9">
-        <v>8449773452</v>
-      </c>
-      <c r="G35" s="1">
-        <v>179</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>289</v>
+        <v>9677</v>
+      </c>
+      <c r="G35" s="9">
+        <v>132</v>
+      </c>
+      <c r="I35" t="s">
+        <v>277</v>
       </c>
       <c r="J35" t="s">
-        <v>296</v>
+        <v>244</v>
       </c>
       <c r="K35" t="s">
         <v>245</v>
       </c>
-      <c r="O35" s="29"/>
-      <c r="P35" s="29"/>
-    </row>
-    <row r="36" spans="1:16">
-      <c r="A36" t="s">
-        <v>209</v>
-      </c>
-      <c r="B36" t="s">
-        <v>338</v>
-      </c>
-      <c r="C36" t="s">
-        <v>290</v>
-      </c>
-      <c r="D36" t="s">
-        <v>201</v>
-      </c>
-      <c r="E36" s="1">
-        <v>34</v>
-      </c>
-      <c r="F36" s="9">
-        <v>605007</v>
-      </c>
-      <c r="G36" s="9">
-        <v>148</v>
-      </c>
-      <c r="I36" t="s">
-        <v>254</v>
-      </c>
-      <c r="J36" t="s">
+    </row>
+    <row r="36" spans="1:16" ht="30">
+      <c r="A36" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="E36" s="27">
+        <v>26</v>
+      </c>
+      <c r="F36" s="23">
+        <v>190807765</v>
+      </c>
+      <c r="G36" s="23">
+        <v>111</v>
+      </c>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="K36" t="s">
-        <v>245</v>
-      </c>
-      <c r="M36" t="s">
-        <v>305</v>
-      </c>
-      <c r="O36" s="29"/>
-      <c r="P36" s="29"/>
+      <c r="K36" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="L36" s="24" t="s">
+        <v>351</v>
+      </c>
+      <c r="M36" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="N36" s="21"/>
     </row>
     <row r="37" spans="1:16">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
         <v>338</v>
@@ -6135,33 +6095,31 @@
       <c r="D37" t="s">
         <v>201</v>
       </c>
-      <c r="E37" s="1">
-        <v>34</v>
-      </c>
-      <c r="F37" s="1">
-        <v>53010</v>
-      </c>
-      <c r="G37" s="1">
-        <v>150</v>
+      <c r="E37" s="12">
+        <v>28</v>
+      </c>
+      <c r="F37" s="9">
+        <v>255521795</v>
+      </c>
+      <c r="G37" s="9">
+        <v>328</v>
       </c>
       <c r="I37" t="s">
-        <v>270</v>
+        <v>287</v>
       </c>
       <c r="J37" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K37" t="s">
         <v>245</v>
       </c>
       <c r="M37" t="s">
-        <v>324</v>
-      </c>
-      <c r="O37" s="29"/>
-      <c r="P37" s="29"/>
+        <v>303</v>
+      </c>
     </row>
     <row r="38" spans="1:16">
       <c r="A38" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="B38" t="s">
         <v>338</v>
@@ -6173,16 +6131,16 @@
         <v>201</v>
       </c>
       <c r="E38" s="1">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F38" s="9">
-        <v>157692631</v>
+        <v>116198466</v>
       </c>
       <c r="G38" s="9">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="I38" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="J38" t="s">
         <v>244</v>
@@ -6190,12 +6148,13 @@
       <c r="K38" t="s">
         <v>245</v>
       </c>
-      <c r="O38" s="29"/>
-      <c r="P38" s="29"/>
+      <c r="M38" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" t="s">
-        <v>217</v>
+        <v>271</v>
       </c>
       <c r="B39" t="s">
         <v>338</v>
@@ -6206,17 +6165,17 @@
       <c r="D39" t="s">
         <v>201</v>
       </c>
-      <c r="E39" s="10">
-        <v>38</v>
-      </c>
-      <c r="F39" s="10">
-        <v>568433400</v>
-      </c>
-      <c r="G39" s="10">
-        <v>147</v>
+      <c r="E39" s="1">
+        <v>30</v>
+      </c>
+      <c r="F39" s="1">
+        <v>37093353</v>
+      </c>
+      <c r="G39" s="1">
+        <v>59</v>
       </c>
       <c r="I39" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="J39" t="s">
         <v>244</v>
@@ -6224,161 +6183,148 @@
       <c r="K39" t="s">
         <v>245</v>
       </c>
-      <c r="M39" t="s">
-        <v>308</v>
-      </c>
-      <c r="O39" s="29"/>
-      <c r="P39" s="29"/>
-    </row>
-    <row r="40" spans="1:16">
-      <c r="A40" t="s">
-        <v>226</v>
-      </c>
-      <c r="B40" t="s">
+    </row>
+    <row r="40" spans="1:16" ht="30">
+      <c r="A40" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="E40" s="22">
+        <v>31</v>
+      </c>
+      <c r="F40" s="23">
+        <v>867535</v>
+      </c>
+      <c r="G40" s="23">
+        <v>354</v>
+      </c>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="K40" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="L40" s="28" t="s">
+        <v>346</v>
+      </c>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+    </row>
+    <row r="41" spans="1:16" ht="30">
+      <c r="A41" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="E41" s="26">
+        <v>31</v>
+      </c>
+      <c r="F41" s="26">
+        <v>6797842</v>
+      </c>
+      <c r="G41" s="26">
+        <v>157</v>
+      </c>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="K41" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="L41" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="M41" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="N41" s="21"/>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
         <v>338</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>290</v>
       </c>
-      <c r="D40" t="s">
-        <v>201</v>
-      </c>
-      <c r="E40" s="1">
-        <v>38</v>
-      </c>
-      <c r="F40" s="9">
-        <v>179453</v>
-      </c>
-      <c r="G40" s="9">
-        <v>161</v>
-      </c>
-      <c r="I40" t="s">
-        <v>264</v>
-      </c>
-      <c r="J40" t="s">
+      <c r="D42" t="s">
+        <v>201</v>
+      </c>
+      <c r="E42" s="10">
+        <v>32</v>
+      </c>
+      <c r="F42" s="9">
+        <v>8449773452</v>
+      </c>
+      <c r="G42" s="1">
+        <v>179</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="J42" t="s">
+        <v>296</v>
+      </c>
+      <c r="K42" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="E43" s="22">
+        <v>32</v>
+      </c>
+      <c r="F43" s="23">
+        <v>21937596</v>
+      </c>
+      <c r="G43" s="23">
+        <v>77</v>
+      </c>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="K40" t="s">
-        <v>245</v>
-      </c>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-    </row>
-    <row r="41" spans="1:16">
-      <c r="A41" t="s">
-        <v>224</v>
-      </c>
-      <c r="B41" t="s">
-        <v>338</v>
-      </c>
-      <c r="C41" t="s">
-        <v>290</v>
-      </c>
-      <c r="D41" t="s">
-        <v>201</v>
-      </c>
-      <c r="E41" s="12">
-        <v>41</v>
-      </c>
-      <c r="F41" s="12">
-        <v>43522</v>
-      </c>
-      <c r="G41" s="12">
-        <v>136</v>
-      </c>
-      <c r="H41" t="s">
-        <v>225</v>
-      </c>
-      <c r="I41" t="s">
-        <v>259</v>
-      </c>
-      <c r="J41" t="s">
-        <v>244</v>
-      </c>
-      <c r="K41" t="s">
-        <v>245</v>
-      </c>
-      <c r="M41" t="s">
-        <v>315</v>
-      </c>
-      <c r="O41" s="29"/>
-      <c r="P41" s="29"/>
-    </row>
-    <row r="42" spans="1:16" s="29" customFormat="1">
-      <c r="A42" s="29" t="s">
-        <v>234</v>
-      </c>
-      <c r="B42" s="29" t="s">
-        <v>338</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E42" s="30">
-        <v>45</v>
-      </c>
-      <c r="F42" s="33">
-        <v>2628415</v>
-      </c>
-      <c r="G42" s="33">
-        <v>189</v>
-      </c>
-      <c r="I42" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="J42" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="K42" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="L42" s="32"/>
-      <c r="M42" s="29" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" s="29" customFormat="1">
-      <c r="A43" s="29" t="s">
-        <v>228</v>
-      </c>
-      <c r="B43" s="29" t="s">
-        <v>338</v>
-      </c>
-      <c r="C43" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="D43" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E43" s="31">
-        <v>47</v>
-      </c>
-      <c r="F43" s="31">
-        <v>10573921</v>
-      </c>
-      <c r="G43" s="31">
-        <v>260</v>
-      </c>
-      <c r="I43" s="29" t="s">
-        <v>273</v>
-      </c>
-      <c r="J43" s="29" t="s">
-        <v>298</v>
-      </c>
-      <c r="K43" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="L43" s="32"/>
-      <c r="M43" s="29" t="s">
-        <v>323</v>
-      </c>
+      <c r="K43" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="L43" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
+      <c r="P43" s="21"/>
     </row>
     <row r="44" spans="1:16">
       <c r="A44" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B44" t="s">
         <v>338</v>
@@ -6390,16 +6336,16 @@
         <v>201</v>
       </c>
       <c r="E44" s="1">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F44" s="9">
-        <v>276204</v>
+        <v>605007</v>
       </c>
       <c r="G44" s="9">
-        <v>315</v>
+        <v>148</v>
       </c>
       <c r="I44" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="J44" t="s">
         <v>244</v>
@@ -6408,12 +6354,12 @@
         <v>245</v>
       </c>
       <c r="M44" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="45" spans="1:16">
       <c r="A45" t="s">
-        <v>227</v>
+        <v>159</v>
       </c>
       <c r="B45" t="s">
         <v>338</v>
@@ -6424,47 +6370,49 @@
       <c r="D45" t="s">
         <v>201</v>
       </c>
-      <c r="E45" s="12">
-        <v>49</v>
-      </c>
-      <c r="F45" s="9">
-        <v>3517803045</v>
-      </c>
-      <c r="G45" s="9">
-        <v>177</v>
-      </c>
-      <c r="I45" s="8" t="s">
-        <v>349</v>
+      <c r="E45" s="1">
+        <v>34</v>
+      </c>
+      <c r="F45" s="1">
+        <v>53010</v>
+      </c>
+      <c r="G45" s="1">
+        <v>150</v>
+      </c>
+      <c r="I45" t="s">
+        <v>270</v>
       </c>
       <c r="J45" t="s">
-        <v>244</v>
+        <v>298</v>
       </c>
       <c r="K45" t="s">
         <v>245</v>
       </c>
       <c r="M45" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="30">
       <c r="A46" s="21" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B46" s="21" t="s">
         <v>353</v>
       </c>
-      <c r="C46" s="21"/>
+      <c r="C46" s="21" t="s">
+        <v>290</v>
+      </c>
       <c r="D46" s="21" t="s">
         <v>201</v>
       </c>
       <c r="E46" s="22">
-        <v>15</v>
-      </c>
-      <c r="F46" s="22">
-        <v>6148355</v>
-      </c>
-      <c r="G46" s="22">
-        <v>57</v>
+        <v>35</v>
+      </c>
+      <c r="F46" s="23">
+        <v>61545575</v>
+      </c>
+      <c r="G46" s="23">
+        <v>156</v>
       </c>
       <c r="H46" s="21"/>
       <c r="I46" s="21"/>
@@ -6474,17 +6422,17 @@
       <c r="K46" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="L46" s="24" t="s">
-        <v>344</v>
+      <c r="L46" s="28" t="s">
+        <v>340</v>
       </c>
       <c r="M46" s="21" t="s">
-        <v>329</v>
+        <v>295</v>
       </c>
       <c r="N46" s="21"/>
     </row>
     <row r="47" spans="1:16" ht="30">
       <c r="A47" s="21" t="s">
-        <v>207</v>
+        <v>240</v>
       </c>
       <c r="B47" s="21" t="s">
         <v>353</v>
@@ -6494,13 +6442,13 @@
         <v>201</v>
       </c>
       <c r="E47" s="25">
-        <v>16</v>
-      </c>
-      <c r="F47" s="23">
-        <v>93698</v>
-      </c>
-      <c r="G47" s="23">
-        <v>53</v>
+        <v>36</v>
+      </c>
+      <c r="F47" s="25">
+        <v>224764</v>
+      </c>
+      <c r="G47" s="25">
+        <v>130</v>
       </c>
       <c r="H47" s="21"/>
       <c r="I47" s="21"/>
@@ -6514,115 +6462,117 @@
         <v>344</v>
       </c>
       <c r="M47" s="21" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="N47" s="21"/>
     </row>
-    <row r="48" spans="1:16" ht="30">
-      <c r="A48" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>353</v>
-      </c>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="E48" s="25">
-        <v>18</v>
-      </c>
-      <c r="F48" s="25">
-        <v>1689698</v>
-      </c>
-      <c r="G48" s="25">
-        <v>43</v>
-      </c>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
-      <c r="J48" s="21" t="s">
+    <row r="48" spans="1:16">
+      <c r="A48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B48" t="s">
+        <v>338</v>
+      </c>
+      <c r="C48" t="s">
+        <v>290</v>
+      </c>
+      <c r="D48" t="s">
+        <v>201</v>
+      </c>
+      <c r="E48" s="1">
+        <v>37</v>
+      </c>
+      <c r="F48" s="9">
+        <v>157692631</v>
+      </c>
+      <c r="G48" s="9">
+        <v>174</v>
+      </c>
+      <c r="I48" t="s">
+        <v>275</v>
+      </c>
+      <c r="J48" t="s">
         <v>244</v>
       </c>
-      <c r="K48" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="L48" s="24" t="s">
-        <v>343</v>
-      </c>
-      <c r="M48" s="21"/>
-      <c r="N48" s="21"/>
-    </row>
-    <row r="49" spans="1:14" s="21" customFormat="1" ht="30">
-      <c r="A49" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="B49" s="21" t="s">
-        <v>353</v>
-      </c>
-      <c r="D49" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="E49" s="25">
-        <v>24</v>
-      </c>
-      <c r="F49" s="23">
-        <v>233836</v>
-      </c>
-      <c r="G49" s="23">
-        <v>106</v>
-      </c>
-      <c r="J49" s="21" t="s">
+      <c r="K48" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" s="21" customFormat="1">
+      <c r="A49" t="s">
+        <v>217</v>
+      </c>
+      <c r="B49" t="s">
+        <v>338</v>
+      </c>
+      <c r="C49" t="s">
+        <v>290</v>
+      </c>
+      <c r="D49" t="s">
+        <v>201</v>
+      </c>
+      <c r="E49" s="10">
+        <v>38</v>
+      </c>
+      <c r="F49" s="10">
+        <v>568433400</v>
+      </c>
+      <c r="G49" s="10">
+        <v>147</v>
+      </c>
+      <c r="H49"/>
+      <c r="I49" t="s">
+        <v>258</v>
+      </c>
+      <c r="J49" t="s">
         <v>244</v>
       </c>
-      <c r="K49" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="L49" s="24" t="s">
-        <v>344</v>
-      </c>
-      <c r="M49" s="21" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" ht="30">
-      <c r="A50" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="B50" s="21" t="s">
-        <v>353</v>
-      </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="E50" s="27">
-        <v>26</v>
-      </c>
-      <c r="F50" s="23">
-        <v>190807765</v>
-      </c>
-      <c r="G50" s="23">
-        <v>111</v>
-      </c>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21" t="s">
+      <c r="K49" t="s">
+        <v>245</v>
+      </c>
+      <c r="L49" s="20"/>
+      <c r="M49" t="s">
+        <v>308</v>
+      </c>
+      <c r="N49"/>
+      <c r="O49"/>
+      <c r="P49"/>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="A50" t="s">
+        <v>226</v>
+      </c>
+      <c r="B50" t="s">
+        <v>338</v>
+      </c>
+      <c r="C50" t="s">
+        <v>290</v>
+      </c>
+      <c r="D50" t="s">
+        <v>201</v>
+      </c>
+      <c r="E50" s="1">
+        <v>38</v>
+      </c>
+      <c r="F50" s="9">
+        <v>179453</v>
+      </c>
+      <c r="G50" s="9">
+        <v>161</v>
+      </c>
+      <c r="I50" t="s">
+        <v>264</v>
+      </c>
+      <c r="J50" t="s">
         <v>244</v>
       </c>
-      <c r="K50" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="L50" s="24" t="s">
-        <v>351</v>
-      </c>
-      <c r="M50" s="21" t="s">
-        <v>311</v>
-      </c>
-      <c r="N50" s="21"/>
-    </row>
-    <row r="51" spans="1:14" ht="30">
+      <c r="K50" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="30">
       <c r="A51" s="21" t="s">
-        <v>143</v>
+        <v>202</v>
       </c>
       <c r="B51" s="21" t="s">
         <v>353</v>
@@ -6632,67 +6582,73 @@
         <v>201</v>
       </c>
       <c r="E51" s="22">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F51" s="23">
-        <v>867535</v>
+        <v>612439379</v>
       </c>
       <c r="G51" s="23">
-        <v>354</v>
+        <v>886</v>
       </c>
       <c r="H51" s="21"/>
-      <c r="I51" s="21"/>
+      <c r="I51" s="21" t="s">
+        <v>336</v>
+      </c>
       <c r="J51" s="21" t="s">
         <v>296</v>
       </c>
       <c r="K51" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="L51" s="28" t="s">
-        <v>346</v>
-      </c>
-      <c r="M51" s="21"/>
+      <c r="L51" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="M51" s="21" t="s">
+        <v>297</v>
+      </c>
       <c r="N51" s="21"/>
     </row>
-    <row r="52" spans="1:14" ht="30">
-      <c r="A52" s="21" t="s">
-        <v>345</v>
-      </c>
-      <c r="B52" s="21" t="s">
-        <v>353</v>
-      </c>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="E52" s="26">
-        <v>31</v>
-      </c>
-      <c r="F52" s="26">
-        <v>6797842</v>
-      </c>
-      <c r="G52" s="26">
-        <v>157</v>
-      </c>
-      <c r="H52" s="21"/>
-      <c r="I52" s="21"/>
-      <c r="J52" s="21" t="s">
+    <row r="52" spans="1:16">
+      <c r="A52" t="s">
+        <v>224</v>
+      </c>
+      <c r="B52" t="s">
+        <v>338</v>
+      </c>
+      <c r="C52" t="s">
+        <v>290</v>
+      </c>
+      <c r="D52" t="s">
+        <v>201</v>
+      </c>
+      <c r="E52" s="12">
+        <v>41</v>
+      </c>
+      <c r="F52" s="12">
+        <v>43522</v>
+      </c>
+      <c r="G52" s="12">
+        <v>136</v>
+      </c>
+      <c r="H52" t="s">
+        <v>225</v>
+      </c>
+      <c r="I52" t="s">
+        <v>259</v>
+      </c>
+      <c r="J52" t="s">
         <v>244</v>
       </c>
-      <c r="K52" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="L52" s="24" t="s">
-        <v>344</v>
-      </c>
-      <c r="M52" s="21" t="s">
-        <v>325</v>
-      </c>
-      <c r="N52" s="21"/>
-    </row>
-    <row r="53" spans="1:14" ht="30">
+      <c r="K52" t="s">
+        <v>245</v>
+      </c>
+      <c r="M52" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53" s="21" t="s">
-        <v>189</v>
+        <v>223</v>
       </c>
       <c r="B53" s="21" t="s">
         <v>353</v>
@@ -6703,70 +6659,69 @@
       <c r="D53" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="E53" s="22">
-        <v>35</v>
+      <c r="E53" s="25">
+        <v>42</v>
       </c>
       <c r="F53" s="23">
-        <v>61545575</v>
+        <v>470254737</v>
       </c>
       <c r="G53" s="23">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="H53" s="21"/>
       <c r="I53" s="21"/>
       <c r="J53" s="21" t="s">
-        <v>294</v>
+        <v>244</v>
       </c>
       <c r="K53" s="21" t="s">
         <v>248</v>
       </c>
       <c r="L53" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M53" s="21" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
       <c r="N53" s="21"/>
     </row>
-    <row r="54" spans="1:14" ht="30">
-      <c r="A54" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="B54" s="21" t="s">
-        <v>353</v>
-      </c>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="E54" s="25">
-        <v>36</v>
-      </c>
-      <c r="F54" s="25">
-        <v>224764</v>
-      </c>
-      <c r="G54" s="25">
-        <v>130</v>
-      </c>
-      <c r="H54" s="21"/>
-      <c r="I54" s="21"/>
-      <c r="J54" s="21" t="s">
+    <row r="54" spans="1:16">
+      <c r="A54" t="s">
+        <v>234</v>
+      </c>
+      <c r="B54" t="s">
+        <v>338</v>
+      </c>
+      <c r="C54" t="s">
+        <v>290</v>
+      </c>
+      <c r="D54" t="s">
+        <v>201</v>
+      </c>
+      <c r="E54" s="1">
+        <v>45</v>
+      </c>
+      <c r="F54" s="9">
+        <v>2628415</v>
+      </c>
+      <c r="G54" s="9">
+        <v>189</v>
+      </c>
+      <c r="I54" t="s">
+        <v>276</v>
+      </c>
+      <c r="J54" t="s">
         <v>244</v>
       </c>
-      <c r="K54" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="L54" s="24" t="s">
-        <v>344</v>
-      </c>
-      <c r="M54" s="21" t="s">
-        <v>335</v>
-      </c>
-      <c r="N54" s="21"/>
-    </row>
-    <row r="55" spans="1:14" ht="30">
+      <c r="K54" t="s">
+        <v>245</v>
+      </c>
+      <c r="M54" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="30">
       <c r="A55" s="21" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="B55" s="21" t="s">
         <v>353</v>
@@ -6775,21 +6730,19 @@
       <c r="D55" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="E55" s="22">
-        <v>38</v>
-      </c>
-      <c r="F55" s="23">
-        <v>612439379</v>
-      </c>
-      <c r="G55" s="23">
-        <v>886</v>
+      <c r="E55" s="26">
+        <v>45</v>
+      </c>
+      <c r="F55" s="26">
+        <v>19152251</v>
+      </c>
+      <c r="G55" s="26">
+        <v>184</v>
       </c>
       <c r="H55" s="21"/>
-      <c r="I55" s="21" t="s">
-        <v>336</v>
-      </c>
+      <c r="I55" s="21"/>
       <c r="J55" s="21" t="s">
-        <v>296</v>
+        <v>244</v>
       </c>
       <c r="K55" s="21" t="s">
         <v>248</v>
@@ -6798,127 +6751,121 @@
         <v>344</v>
       </c>
       <c r="M55" s="21" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="N55" s="21"/>
     </row>
-    <row r="56" spans="1:14">
-      <c r="A56" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="B56" s="21" t="s">
+    <row r="56" spans="1:16">
+      <c r="A56" t="s">
+        <v>228</v>
+      </c>
+      <c r="B56" t="s">
+        <v>338</v>
+      </c>
+      <c r="C56" t="s">
+        <v>290</v>
+      </c>
+      <c r="D56" t="s">
+        <v>201</v>
+      </c>
+      <c r="E56" s="10">
+        <v>47</v>
+      </c>
+      <c r="F56" s="10">
+        <v>10573921</v>
+      </c>
+      <c r="G56" s="10">
+        <v>260</v>
+      </c>
+      <c r="I56" t="s">
+        <v>273</v>
+      </c>
+      <c r="J56" t="s">
+        <v>298</v>
+      </c>
+      <c r="K56" t="s">
+        <v>245</v>
+      </c>
+      <c r="M56" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="A57" t="s">
+        <v>210</v>
+      </c>
+      <c r="B57" t="s">
+        <v>338</v>
+      </c>
+      <c r="C57" t="s">
+        <v>290</v>
+      </c>
+      <c r="D57" t="s">
+        <v>201</v>
+      </c>
+      <c r="E57" s="1">
+        <v>48</v>
+      </c>
+      <c r="F57" s="9">
+        <v>276204</v>
+      </c>
+      <c r="G57" s="9">
+        <v>315</v>
+      </c>
+      <c r="I57" t="s">
+        <v>253</v>
+      </c>
+      <c r="J57" t="s">
+        <v>244</v>
+      </c>
+      <c r="K57" t="s">
+        <v>245</v>
+      </c>
+      <c r="M57" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="A58" t="s">
+        <v>227</v>
+      </c>
+      <c r="B58" t="s">
+        <v>338</v>
+      </c>
+      <c r="C58" t="s">
+        <v>290</v>
+      </c>
+      <c r="D58" t="s">
+        <v>201</v>
+      </c>
+      <c r="E58" s="12">
+        <v>49</v>
+      </c>
+      <c r="F58" s="9">
+        <v>3517803045</v>
+      </c>
+      <c r="G58" s="9">
+        <v>177</v>
+      </c>
+      <c r="I58" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="J58" t="s">
+        <v>244</v>
+      </c>
+      <c r="K58" t="s">
+        <v>245</v>
+      </c>
+      <c r="M58" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" s="21" customFormat="1" ht="30">
+      <c r="A59" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B59" s="21" t="s">
         <v>353</v>
-      </c>
-      <c r="C56" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="D56" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="E56" s="25">
-        <v>42</v>
-      </c>
-      <c r="F56" s="23">
-        <v>470254737</v>
-      </c>
-      <c r="G56" s="23">
-        <v>129</v>
-      </c>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="21" t="s">
-        <v>244</v>
-      </c>
-      <c r="K56" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="L56" s="28" t="s">
-        <v>339</v>
-      </c>
-      <c r="M56" s="21" t="s">
-        <v>314</v>
-      </c>
-      <c r="N56" s="21"/>
-    </row>
-    <row r="57" spans="1:14" ht="30">
-      <c r="A57" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="B57" s="21" t="s">
-        <v>353</v>
-      </c>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="E57" s="26">
-        <v>45</v>
-      </c>
-      <c r="F57" s="26">
-        <v>19152251</v>
-      </c>
-      <c r="G57" s="26">
-        <v>184</v>
-      </c>
-      <c r="H57" s="21"/>
-      <c r="I57" s="21"/>
-      <c r="J57" s="21" t="s">
-        <v>244</v>
-      </c>
-      <c r="K57" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="L57" s="24" t="s">
-        <v>344</v>
-      </c>
-      <c r="M57" s="21" t="s">
-        <v>310</v>
-      </c>
-      <c r="N57" s="21"/>
-    </row>
-    <row r="58" spans="1:14" ht="30">
-      <c r="A58" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B58" s="21" t="s">
-        <v>353</v>
-      </c>
-      <c r="C58" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="D58" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="E58" s="22">
-        <v>51</v>
-      </c>
-      <c r="F58" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="G58" s="23">
-        <v>315</v>
-      </c>
-      <c r="H58" s="21"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="21" t="s">
-        <v>298</v>
-      </c>
-      <c r="K58" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="L58" s="28" t="s">
-        <v>341</v>
-      </c>
-      <c r="M58" s="21" t="s">
-        <v>299</v>
-      </c>
-      <c r="N58" s="21" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" s="21" customFormat="1">
-      <c r="A59" s="21" t="s">
-        <v>215</v>
       </c>
       <c r="C59" s="21" t="s">
         <v>290</v>
@@ -6927,23 +6874,31 @@
         <v>201</v>
       </c>
       <c r="E59" s="22">
-        <v>32</v>
-      </c>
-      <c r="F59" s="23">
-        <v>21937596</v>
+        <v>51</v>
+      </c>
+      <c r="F59" s="23" t="s">
+        <v>88</v>
       </c>
       <c r="G59" s="23">
-        <v>77</v>
+        <v>315</v>
       </c>
       <c r="J59" s="21" t="s">
-        <v>244</v>
+        <v>298</v>
       </c>
       <c r="K59" s="21" t="s">
         <v>248</v>
       </c>
       <c r="L59" s="28" t="s">
-        <v>339</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="M59" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="N59" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="O59"/>
+      <c r="P59"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:N59" xr:uid="{00000000-0009-0000-0000-000005000000}">
@@ -6952,62 +6907,65 @@
       <sortCondition ref="E2:E59"/>
     </sortState>
   </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P59">
+    <sortCondition ref="E2:E59"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="A28" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="A5" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="A31" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
     <hyperlink ref="A14" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="A35" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="A38" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="A10" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="A47" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="A32" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="A50" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="A49" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-    <hyperlink ref="A45" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
-    <hyperlink ref="A7" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
-    <hyperlink ref="A55" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
-    <hyperlink ref="A43" r:id="rId14" xr:uid="{00000000-0004-0000-0500-00000D000000}"/>
-    <hyperlink ref="A54" r:id="rId15" xr:uid="{00000000-0004-0000-0500-00000E000000}"/>
-    <hyperlink ref="A57" r:id="rId16" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
-    <hyperlink ref="A52" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
-    <hyperlink ref="A39" r:id="rId18" xr:uid="{00000000-0004-0000-0500-000011000000}"/>
+    <hyperlink ref="A42" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="A48" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="A9" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="A18" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="A37" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="A36" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="A34" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="A58" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
+    <hyperlink ref="A6" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
+    <hyperlink ref="A51" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
+    <hyperlink ref="A56" r:id="rId14" xr:uid="{00000000-0004-0000-0500-00000D000000}"/>
+    <hyperlink ref="A47" r:id="rId15" xr:uid="{00000000-0004-0000-0500-00000E000000}"/>
+    <hyperlink ref="A55" r:id="rId16" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
+    <hyperlink ref="A41" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
+    <hyperlink ref="A49" r:id="rId18" xr:uid="{00000000-0004-0000-0500-000011000000}"/>
     <hyperlink ref="A15" r:id="rId19" xr:uid="{00000000-0004-0000-0500-000012000000}"/>
-    <hyperlink ref="A48" r:id="rId20" xr:uid="{00000000-0004-0000-0500-000013000000}"/>
-    <hyperlink ref="A13" r:id="rId21" xr:uid="{00000000-0004-0000-0500-000014000000}"/>
-    <hyperlink ref="A41" r:id="rId22" xr:uid="{00000000-0004-0000-0500-000015000000}"/>
-    <hyperlink ref="A34" r:id="rId23" xr:uid="{00000000-0004-0000-0500-000016000000}"/>
-    <hyperlink ref="A36" r:id="rId24" xr:uid="{00000000-0004-0000-0500-000017000000}"/>
-    <hyperlink ref="A56" r:id="rId25" xr:uid="{00000000-0004-0000-0500-000018000000}"/>
-    <hyperlink ref="A9" r:id="rId26" xr:uid="{00000000-0004-0000-0500-000019000000}"/>
-    <hyperlink ref="A17" r:id="rId27" xr:uid="{00000000-0004-0000-0500-00001A000000}"/>
-    <hyperlink ref="A30" r:id="rId28" xr:uid="{00000000-0004-0000-0500-00001B000000}"/>
-    <hyperlink ref="A4" r:id="rId29" xr:uid="{00000000-0004-0000-0500-00001C000000}"/>
-    <hyperlink ref="A6" r:id="rId30" xr:uid="{00000000-0004-0000-0500-00001D000000}"/>
-    <hyperlink ref="A12" r:id="rId31" xr:uid="{00000000-0004-0000-0500-00001E000000}"/>
-    <hyperlink ref="A2" r:id="rId32" xr:uid="{00000000-0004-0000-0500-00001F000000}"/>
+    <hyperlink ref="A20" r:id="rId20" xr:uid="{00000000-0004-0000-0500-000013000000}"/>
+    <hyperlink ref="A12" r:id="rId21" xr:uid="{00000000-0004-0000-0500-000014000000}"/>
+    <hyperlink ref="A52" r:id="rId22" xr:uid="{00000000-0004-0000-0500-000015000000}"/>
+    <hyperlink ref="A39" r:id="rId23" xr:uid="{00000000-0004-0000-0500-000016000000}"/>
+    <hyperlink ref="A44" r:id="rId24" xr:uid="{00000000-0004-0000-0500-000017000000}"/>
+    <hyperlink ref="A53" r:id="rId25" xr:uid="{00000000-0004-0000-0500-000018000000}"/>
+    <hyperlink ref="A8" r:id="rId26" xr:uid="{00000000-0004-0000-0500-000019000000}"/>
+    <hyperlink ref="A19" r:id="rId27" xr:uid="{00000000-0004-0000-0500-00001A000000}"/>
+    <hyperlink ref="A33" r:id="rId28" xr:uid="{00000000-0004-0000-0500-00001B000000}"/>
+    <hyperlink ref="A3" r:id="rId29" xr:uid="{00000000-0004-0000-0500-00001C000000}"/>
+    <hyperlink ref="A5" r:id="rId30" xr:uid="{00000000-0004-0000-0500-00001D000000}"/>
+    <hyperlink ref="A11" r:id="rId31" xr:uid="{00000000-0004-0000-0500-00001E000000}"/>
+    <hyperlink ref="A13" r:id="rId32" xr:uid="{00000000-0004-0000-0500-00001F000000}"/>
     <hyperlink ref="A16" r:id="rId33" xr:uid="{00000000-0004-0000-0500-000020000000}"/>
-    <hyperlink ref="A46" r:id="rId34" xr:uid="{00000000-0004-0000-0500-000021000000}"/>
-    <hyperlink ref="A18" r:id="rId35" xr:uid="{00000000-0004-0000-0500-000022000000}"/>
-    <hyperlink ref="A19" r:id="rId36" xr:uid="{00000000-0004-0000-0500-000023000000}"/>
-    <hyperlink ref="A20" r:id="rId37" xr:uid="{00000000-0004-0000-0500-000024000000}"/>
-    <hyperlink ref="A23" r:id="rId38" xr:uid="{00000000-0004-0000-0500-000025000000}"/>
-    <hyperlink ref="A24" r:id="rId39" xr:uid="{00000000-0004-0000-0500-000026000000}"/>
-    <hyperlink ref="A25" r:id="rId40" xr:uid="{00000000-0004-0000-0500-000027000000}"/>
-    <hyperlink ref="A27" r:id="rId41" xr:uid="{00000000-0004-0000-0500-000028000000}"/>
-    <hyperlink ref="A37" r:id="rId42" xr:uid="{00000000-0004-0000-0500-000029000000}"/>
-    <hyperlink ref="A53" r:id="rId43" xr:uid="{00000000-0004-0000-0500-00002A000000}"/>
-    <hyperlink ref="A58" r:id="rId44" xr:uid="{00000000-0004-0000-0500-00002B000000}"/>
-    <hyperlink ref="A31" r:id="rId45" xr:uid="{00000000-0004-0000-0500-00002C000000}"/>
-    <hyperlink ref="A42" r:id="rId46" xr:uid="{00000000-0004-0000-0500-00002D000000}"/>
-    <hyperlink ref="A33" r:id="rId47" xr:uid="{00000000-0004-0000-0500-00002E000000}"/>
-    <hyperlink ref="A29" r:id="rId48" xr:uid="{00000000-0004-0000-0500-00002F000000}"/>
-    <hyperlink ref="A40" r:id="rId49" xr:uid="{00000000-0004-0000-0500-000030000000}"/>
-    <hyperlink ref="A8" r:id="rId50" xr:uid="{00000000-0004-0000-0500-000031000000}"/>
-    <hyperlink ref="A26" r:id="rId51" xr:uid="{00000000-0004-0000-0500-000032000000}"/>
-    <hyperlink ref="A3" r:id="rId52" xr:uid="{00000000-0004-0000-0500-000033000000}"/>
-    <hyperlink ref="A51" r:id="rId53" xr:uid="{00000000-0004-0000-0500-000034000000}"/>
-    <hyperlink ref="A21" r:id="rId54" xr:uid="{00000000-0004-0000-0500-000035000000}"/>
-    <hyperlink ref="A44" r:id="rId55" xr:uid="{00000000-0004-0000-0500-000036000000}"/>
+    <hyperlink ref="A17" r:id="rId34" xr:uid="{00000000-0004-0000-0500-000021000000}"/>
+    <hyperlink ref="A21" r:id="rId35" xr:uid="{00000000-0004-0000-0500-000022000000}"/>
+    <hyperlink ref="A22" r:id="rId36" xr:uid="{00000000-0004-0000-0500-000023000000}"/>
+    <hyperlink ref="A23" r:id="rId37" xr:uid="{00000000-0004-0000-0500-000024000000}"/>
+    <hyperlink ref="A26" r:id="rId38" xr:uid="{00000000-0004-0000-0500-000025000000}"/>
+    <hyperlink ref="A27" r:id="rId39" xr:uid="{00000000-0004-0000-0500-000026000000}"/>
+    <hyperlink ref="A28" r:id="rId40" xr:uid="{00000000-0004-0000-0500-000027000000}"/>
+    <hyperlink ref="A30" r:id="rId41" xr:uid="{00000000-0004-0000-0500-000028000000}"/>
+    <hyperlink ref="A45" r:id="rId42" xr:uid="{00000000-0004-0000-0500-000029000000}"/>
+    <hyperlink ref="A46" r:id="rId43" xr:uid="{00000000-0004-0000-0500-00002A000000}"/>
+    <hyperlink ref="A59" r:id="rId44" xr:uid="{00000000-0004-0000-0500-00002B000000}"/>
+    <hyperlink ref="A35" r:id="rId45" xr:uid="{00000000-0004-0000-0500-00002C000000}"/>
+    <hyperlink ref="A54" r:id="rId46" xr:uid="{00000000-0004-0000-0500-00002D000000}"/>
+    <hyperlink ref="A38" r:id="rId47" xr:uid="{00000000-0004-0000-0500-00002E000000}"/>
+    <hyperlink ref="A32" r:id="rId48" xr:uid="{00000000-0004-0000-0500-00002F000000}"/>
+    <hyperlink ref="A50" r:id="rId49" xr:uid="{00000000-0004-0000-0500-000030000000}"/>
+    <hyperlink ref="A7" r:id="rId50" xr:uid="{00000000-0004-0000-0500-000031000000}"/>
+    <hyperlink ref="A29" r:id="rId51" xr:uid="{00000000-0004-0000-0500-000032000000}"/>
+    <hyperlink ref="A2" r:id="rId52" xr:uid="{00000000-0004-0000-0500-000033000000}"/>
+    <hyperlink ref="A40" r:id="rId53" xr:uid="{00000000-0004-0000-0500-000034000000}"/>
+    <hyperlink ref="A24" r:id="rId54" xr:uid="{00000000-0004-0000-0500-000035000000}"/>
+    <hyperlink ref="A57" r:id="rId55" xr:uid="{00000000-0004-0000-0500-000036000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId56"/>

</xml_diff>